<commit_message>
Implement Keyword-Driven framework for isBaseicAuthenticated request
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheets/KeywordsSheet.xlsx
+++ b/src/test/resources/ExcelSheets/KeywordsSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">TC_ID</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">basicAuthentication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tokenAuthentication</t>
   </si>
 </sst>
 </file>
@@ -86,12 +83,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,8 +131,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -142,6 +149,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -153,28 +220,28 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="22.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -195,11 +262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>